<commit_message>
1.data updated; 2.resolve nan error
</commit_message>
<xml_diff>
--- a/inputs/relations.xlsx
+++ b/inputs/relations.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="20475" windowHeight="8730"/>
+    <workbookView windowWidth="15360" windowHeight="7860"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,12 +16,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
   <si>
     <t>CJM622</t>
   </si>
   <si>
+    <t>CJM729</t>
+  </si>
+  <si>
     <t>CJM815</t>
+  </si>
+  <si>
+    <t>CJM911</t>
   </si>
   <si>
     <t>CJM995</t>
@@ -36,48 +42,207 @@
     <t>DM8034</t>
   </si>
   <si>
-    <t>USG</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t>U</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t>SG</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="180" formatCode="#,##0_);[Red]\(#,##0\)"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="5">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="#,##0_);[Red]\(#,##0\)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color indexed="8"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
-      <color indexed="8"/>
+      <color theme="1"/>
       <name val="微软雅黑"/>
-      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="2"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -86,12 +251,198 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF76933C"/>
+        <fgColor theme="6" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -134,9 +485,251 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -144,23 +737,92 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="176" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -451,212 +1113,279 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H8"/>
+      <selection activeCell="A1" sqref="A1:J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2"/>
-      <c r="B1" s="3" t="s">
+    <row r="1" ht="17.25" spans="1:10">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="I1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="2" ht="17.25" spans="1:10">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="3">
         <v>1</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+    <row r="3" ht="17.25" spans="1:10">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1">
-        <v>0.34488192836960302</v>
-      </c>
-      <c r="C3" s="1">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3">
         <v>1</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+    <row r="4" ht="17.25" spans="1:10">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1">
-        <v>0.22897819144057499</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0.38652007341251998</v>
-      </c>
-      <c r="D4" s="1">
+      <c r="B4" s="3">
+        <v>0.344881928369603</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3">
         <v>1</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+    <row r="5" ht="17.25" spans="1:10">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+    </row>
+    <row r="6" ht="17.25" spans="1:10">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.228978191440575</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3">
+        <v>0.38652007341252</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" ht="17.25" spans="1:10">
+      <c r="A7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3">
         <v>0.110097554573187</v>
       </c>
-      <c r="C5" s="1">
-        <v>0.24060150161799199</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0.21983642530581601</v>
-      </c>
-      <c r="E5" s="1">
+      <c r="C7" s="3"/>
+      <c r="D7" s="3">
+        <v>0.240601501617992</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3">
+        <v>0.219836425305816</v>
+      </c>
+      <c r="G7" s="3">
         <v>1</v>
       </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
     </row>
-    <row r="6" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0.92966532823327697</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0.35885029500698801</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0.37337083532725901</v>
-      </c>
-      <c r="E6" s="1">
-        <v>9.3812524489076302E-2</v>
-      </c>
-      <c r="F6" s="1">
+    <row r="8" ht="17.25" spans="1:10">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.929665328233277</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3">
+        <v>0.358850295006988</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3">
+        <v>0.373370835327259</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0.0938125244890763</v>
+      </c>
+      <c r="H8" s="3">
         <v>1</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
     </row>
-    <row r="7" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1">
-        <v>0.91192237015410904</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0.37931650316246002</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0.46761968787361802</v>
-      </c>
-      <c r="E7" s="1">
-        <v>8.6959170793381793E-2</v>
-      </c>
-      <c r="F7" s="1">
-        <v>0.98266566487553997</v>
-      </c>
-      <c r="G7" s="1">
+    <row r="9" ht="17.25" spans="1:10">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.911922370154109</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3">
+        <v>0.37931650316246</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3">
+        <v>0.467619687873618</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0.0869591707933818</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0.98266566487554</v>
+      </c>
+      <c r="I9" s="3">
         <v>1</v>
       </c>
-      <c r="H7" s="1"/>
+      <c r="J9" s="3"/>
     </row>
-    <row r="8" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="4">
-        <v>0.20929390919740101</v>
-      </c>
-      <c r="C8" s="4">
-        <v>0.22230658324455799</v>
-      </c>
-      <c r="D8" s="4">
-        <v>1.4863705407065201E-2</v>
-      </c>
-      <c r="E8" s="4">
-        <v>-7.5431074857788397E-2</v>
-      </c>
-      <c r="F8" s="4">
-        <v>6.3873116758791801E-2</v>
-      </c>
-      <c r="G8" s="4">
-        <v>7.3433800147775202E-2</v>
-      </c>
-      <c r="H8" s="4">
+    <row r="10" ht="17.25" spans="1:10">
+      <c r="A10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0.209293909197401</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4">
+        <v>0.222306583244558</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4">
+        <v>0.0148637054070652</v>
+      </c>
+      <c r="G10" s="4">
+        <v>-0.0754310748577884</v>
+      </c>
+      <c r="H10" s="4">
+        <v>0.0638731167587918</v>
+      </c>
+      <c r="I10" s="4">
+        <v>0.0734338001477752</v>
+      </c>
+      <c r="J10" s="4">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <conditionalFormatting sqref="B2:J10">
+    <cfRule type="top10" dxfId="0" priority="7" rank="3"/>
+    <cfRule type="top10" dxfId="0" priority="6" rank="8"/>
+    <cfRule type="top10" dxfId="0" priority="5" rank="10"/>
+    <cfRule type="top10" dxfId="0" priority="4" bottom="1" rank="2"/>
+    <cfRule type="top10" dxfId="1" priority="3" bottom="1" rank="2"/>
+    <cfRule type="top10" dxfId="0" priority="2" bottom="1" rank="4"/>
+    <cfRule type="top10" dxfId="1" priority="1" bottom="1" rank="6"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
-  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
-  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>